<commit_message>
Attendance & Forms System
[Attendance]
-Set unassigned names to "Unassigned" instead of showing "None, None, N."
[Forms]
-Write male counter when exporting for SF5
</commit_message>
<xml_diff>
--- a/Sample Data/Task Checklist.xlsx
+++ b/Sample Data/Task Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pader\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\CBNHS-System\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E94BFF-A01C-4C08-88AD-3134E314DB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1888D7C1-64DA-422D-B84B-9863F0D2A2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{F06D959A-A747-46A5-9DFC-5634EE2C6498}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="3" xr2:uid="{F06D959A-A747-46A5-9DFC-5634EE2C6498}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-enrollment" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="73">
   <si>
     <t>Tasks</t>
   </si>
@@ -242,6 +242,13 @@
   </si>
   <si>
     <t>SF6</t>
+  </si>
+  <si>
+    <t>Generate Grades for General Average(Optional)</t>
+  </si>
+  <si>
+    <t>Generate Grades for General Average
+(Optional Unless Final Quarter)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -310,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6277AC-17F6-429B-9748-B623885D606D}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -898,103 +908,107 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9BE3E8-FFDC-4FF3-8D0A-22B7A3DB5E3F}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E5" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C8"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1004,52 +1018,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939E37F5-414C-45F9-8275-6C91DFF93525}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1057,62 +1071,67 @@
       <c r="B3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="9" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C10"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Task checklist fonts
</commit_message>
<xml_diff>
--- a/Sample Data/Task Checklist.xlsx
+++ b/Sample Data/Task Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\CBNHS-System\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1888D7C1-64DA-422D-B84B-9863F0D2A2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2A3410-2E6B-4FB9-A0F1-4BC237EB8FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="3" xr2:uid="{F06D959A-A747-46A5-9DFC-5634EE2C6498}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{F06D959A-A747-46A5-9DFC-5634EE2C6498}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-enrollment" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Transferees &amp; Old Students</t>
   </si>
   <si>
-    <t>Import Existing students' Data (Optional)</t>
-  </si>
-  <si>
     <t>Enroll students to their respective section based on the School's criteria of admittance</t>
   </si>
   <si>
@@ -249,13 +246,16 @@
   <si>
     <t>Generate Grades for General Average
 (Optional Unless Final Quarter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import Existing students' Data </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,9 +267,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -280,7 +285,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -288,38 +293,157 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,200 +761,245 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6277AC-17F6-429B-9748-B623885D606D}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="14" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -840,65 +1009,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CE665-7120-49C4-A8CB-59359C0B8DE1}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -908,107 +1092,137 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9BE3E8-FFDC-4FF3-8D0A-22B7A3DB5E3F}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="E7" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1018,247 +1232,330 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939E37F5-414C-45F9-8275-6C91DFF93525}">
-  <dimension ref="A1:E11"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="72" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB1F4DC-0ED6-41B5-844D-03A508E256AC}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>